<commit_message>
Filter2 - second channel - wip
</commit_message>
<xml_diff>
--- a/modules/Filter2/positions.xlsx
+++ b/modules/Filter2/positions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Filter2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D4DA88-FA32-44FB-A4ED-CC438B08A92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4557DE4-8C0E-4688-BC2E-AB64EC4E35F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="1290" windowWidth="18540" windowHeight="12495" xr2:uid="{7A854C23-8C7F-43C5-86C4-846A5F5DE0F0}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,21 +444,23 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>4.2413385830000001</v>
+        <f>4.34+0.1</f>
+        <v>4.4399999999999995</v>
       </c>
       <c r="C2">
-        <v>5.137007874</v>
+        <f>5.235433071+0.1</f>
+        <v>5.3354330709999997</v>
       </c>
       <c r="D2">
-        <v>1.9</v>
+        <v>1.508</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>4.2413385830000001</v>
@@ -472,7 +474,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>4.2413385830000001</v>
@@ -486,19 +488,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <f>4.34+0.1</f>
-        <v>4.4399999999999995</v>
+        <v>4.2413385830000001</v>
       </c>
       <c r="C5">
-        <f>5.235433071+0.1</f>
-        <v>5.3354330709999997</v>
+        <v>5.137007874</v>
       </c>
       <c r="D5">
-        <f>3.854724409-0.1</f>
-        <v>3.754724409</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>